<commit_message>
latest results for primer paper
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSIR_Scenario0_Primer_200_gaussian.xlsx
+++ b/results/primer/VanillaSIR_Scenario0_Primer_200_gaussian.xlsx
@@ -535,19 +535,19 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2">
-        <v>0.3346278947282513</v>
+        <v>0.3351768771135573</v>
       </c>
       <c r="B2">
-        <v>0.5036053734514618</v>
+        <v>0.5060638175655189</v>
       </c>
       <c r="C2">
-        <v>0.1800088173594993</v>
+        <v>0.1796546986643375</v>
       </c>
       <c r="D2">
-        <v>0.4175805457661747</v>
+        <v>0.4195427544048741</v>
       </c>
       <c r="E2">
-        <v>0.244465865549312</v>
+        <v>0.245578189146106</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -565,64 +565,64 @@
         <v>7</v>
       </c>
       <c r="K2">
-        <v>2.342395263097759</v>
+        <v>2.346238139794901</v>
       </c>
       <c r="L2">
-        <v>3.525237614160233</v>
+        <v>3.542446722958632</v>
       </c>
       <c r="M2">
-        <v>1.260061721516495</v>
+        <v>1.257582890650363</v>
       </c>
       <c r="N2">
-        <v>2.923063820363223</v>
+        <v>2.936799280834118</v>
       </c>
       <c r="O2">
-        <v>1.711261058845184</v>
+        <v>1.719047324022742</v>
       </c>
       <c r="P2">
-        <v>66.9208</v>
+        <v>66.71236</v>
       </c>
       <c r="Q2">
-        <v>160.448613723413</v>
+        <v>158.8199294437367</v>
       </c>
       <c r="R2">
-        <v>-0.5727475235148211</v>
+        <v>-0.9222002297039863</v>
       </c>
       <c r="S2">
-        <v>94.73424782582423</v>
+        <v>93.94103923246006</v>
       </c>
       <c r="T2">
-        <v>41.7674673654717</v>
+        <v>41.68995937282172</v>
       </c>
       <c r="U2">
-        <v>0.2007277116133447</v>
+        <v>0.2013905106781432</v>
       </c>
       <c r="V2">
-        <v>0.3593269136969632</v>
+        <v>0.3608144527543763</v>
       </c>
       <c r="W2">
-        <v>0.01577665778249488</v>
+        <v>0.01761398589523827</v>
       </c>
       <c r="X2">
-        <v>0.2934473879569458</v>
+        <v>0.2937437689855742</v>
       </c>
       <c r="Y2">
-        <v>0.09759430811847805</v>
+        <v>0.09906292406488931</v>
       </c>
       <c r="Z2">
-        <v>0.8048030784860648</v>
+        <v>0.806474547716027</v>
       </c>
       <c r="AA2">
-        <v>1.012458727616161</v>
+        <v>1.013577409345779</v>
       </c>
       <c r="AB2">
-        <v>0.2711897445368369</v>
+        <v>0.2791071634945997</v>
       </c>
       <c r="AC2">
-        <v>0.9052441990640233</v>
+        <v>0.9052320647278638</v>
       </c>
       <c r="AD2">
-        <v>0.618486542944751</v>
+        <v>0.6232276245013814</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -642,171 +642,171 @@
         <v>0.33</v>
       </c>
       <c r="F3">
-        <v>7.031780970968122</v>
+        <v>7.050185388242457</v>
       </c>
       <c r="G3">
-        <v>10.35157562860011</v>
+        <v>10.39984920659461</v>
       </c>
       <c r="H3">
-        <v>3.871631852688999</v>
+        <v>3.86079638696003</v>
       </c>
       <c r="I3">
-        <v>8.681416713841827</v>
+        <v>8.707853521770621</v>
       </c>
       <c r="J3">
-        <v>5.268397729245723</v>
+        <v>5.299282209844216</v>
       </c>
       <c r="K3">
-        <v>2.32048772041948</v>
+        <v>2.326561178120011</v>
       </c>
       <c r="L3">
-        <v>3.416019957438036</v>
+        <v>3.431950238176221</v>
       </c>
       <c r="M3">
-        <v>1.27763851138737</v>
+        <v>1.27406280769681</v>
       </c>
       <c r="N3">
-        <v>2.864867515567803</v>
+        <v>2.873591662184305</v>
       </c>
       <c r="O3">
-        <v>1.738571250651088</v>
+        <v>1.748763129248591</v>
       </c>
       <c r="P3">
-        <v>66.96250000000001</v>
+        <v>66.78951000000001</v>
       </c>
       <c r="Q3">
-        <v>114.242186384998</v>
+        <v>114.5183013445008</v>
       </c>
       <c r="R3">
-        <v>52.35933342789797</v>
+        <v>52.14962197739374</v>
       </c>
       <c r="S3">
-        <v>76.19977862566382</v>
+        <v>75.60569506759896</v>
       </c>
       <c r="T3">
-        <v>56.43118100375168</v>
+        <v>56.39191629479538</v>
       </c>
       <c r="U3">
-        <v>0.1991802249111247</v>
+        <v>0.2001324207050712</v>
       </c>
       <c r="V3">
-        <v>0.347295320366343</v>
+        <v>0.3491814829917947</v>
       </c>
       <c r="W3">
-        <v>0.02976322630320161</v>
+        <v>0.0295351232119927</v>
       </c>
       <c r="X3">
-        <v>0.2859319319833561</v>
+        <v>0.2859781489362377</v>
       </c>
       <c r="Y3">
-        <v>0.1035212279040909</v>
+        <v>0.1052450444196071</v>
       </c>
       <c r="Z3">
-        <v>0.8185561724950173</v>
+        <v>0.8198098386603069</v>
       </c>
       <c r="AA3">
-        <v>0.991718632777663</v>
+        <v>0.9935588253029293</v>
       </c>
       <c r="AB3">
-        <v>0.4184791837534627</v>
+        <v>0.4174250330544992</v>
       </c>
       <c r="AC3">
-        <v>0.9118064114331137</v>
+        <v>0.9111008746823749</v>
       </c>
       <c r="AD3">
-        <v>0.6650093778618686</v>
+        <v>0.6677358467506402</v>
       </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <v>0.3349694863436055</v>
+        <v>0.3350558419577123</v>
       </c>
       <c r="B4">
-        <v>0.5081927706238247</v>
+        <v>0.5086499483008653</v>
       </c>
       <c r="C4">
-        <v>0.1800367434574879</v>
+        <v>0.1800329909208327</v>
       </c>
       <c r="D4">
-        <v>0.420767220842815</v>
+        <v>0.4191459405920589</v>
       </c>
       <c r="E4">
-        <v>0.2448340683946418</v>
+        <v>0.2454954139778766</v>
       </c>
       <c r="F4">
-        <v>7.047104856959494</v>
+        <v>7.053464883417598</v>
       </c>
       <c r="G4">
-        <v>10.37431171480037</v>
+        <v>10.4033846660129</v>
       </c>
       <c r="H4">
-        <v>3.876352708569786</v>
+        <v>3.861647242603307</v>
       </c>
       <c r="I4">
-        <v>8.709815150509453</v>
+        <v>8.702338044188473</v>
       </c>
       <c r="J4">
-        <v>5.311320433757266</v>
+        <v>5.317217194305628</v>
       </c>
       <c r="K4">
-        <v>2.360784270526338</v>
+        <v>2.363622771069657</v>
       </c>
       <c r="L4">
-        <v>4.250342439201584</v>
+        <v>4.233048760917629</v>
       </c>
       <c r="M4">
-        <v>1.035059965818879</v>
+        <v>1.025475250545921</v>
       </c>
       <c r="N4">
-        <v>3.176818680719085</v>
+        <v>3.165455211722798</v>
       </c>
       <c r="O4">
-        <v>1.524953602612467</v>
+        <v>1.518695666687967</v>
       </c>
       <c r="P4">
-        <v>66.5472</v>
+        <v>66.27011</v>
       </c>
       <c r="Q4">
-        <v>162.3423492486556</v>
+        <v>163.82047538298</v>
       </c>
       <c r="R4">
-        <v>0.6612103240337466</v>
+        <v>-0.6129810202759727</v>
       </c>
       <c r="S4">
-        <v>97.7363365788202</v>
+        <v>96.23347761342018</v>
       </c>
       <c r="T4">
-        <v>39.73110595495677</v>
+        <v>39.78443561287411</v>
       </c>
       <c r="U4">
-        <v>0.198175378423829</v>
+        <v>0.1986317842501169</v>
       </c>
       <c r="V4">
-        <v>0.4177151662082227</v>
+        <v>0.4167168209495163</v>
       </c>
       <c r="W4">
-        <v>-0.00808756275911315</v>
+        <v>-0.009228800358541341</v>
       </c>
       <c r="X4">
-        <v>0.3262545874434016</v>
+        <v>0.3265265691653199</v>
       </c>
       <c r="Y4">
-        <v>0.0678901853357273</v>
+        <v>0.06783025487022593</v>
       </c>
       <c r="Z4">
-        <v>0.7668568311167751</v>
+        <v>0.7663562657945971</v>
       </c>
       <c r="AA4">
-        <v>1.026374446992634</v>
+        <v>1.025878516857799</v>
       </c>
       <c r="AB4">
-        <v>0.09015930727236329</v>
+        <v>0.08141683977251001</v>
       </c>
       <c r="AC4">
-        <v>0.9213653488351002</v>
+        <v>0.9214637787715185</v>
       </c>
       <c r="AD4">
-        <v>0.5035562464557588</v>
+        <v>0.500462807955672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>